<commit_message>
Update Ingresos Tributarios 2009-2019.xlsx
</commit_message>
<xml_diff>
--- a/Ingresos tributarios-Impuestos a la renta/Ingresos Tributarios 2009-2019.xlsx
+++ b/Ingresos tributarios-Impuestos a la renta/Ingresos Tributarios 2009-2019.xlsx
@@ -1,44 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f999e057ad8c646/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\DATA INTELLIGENCE Dropbox\Diseño DATA's\DATA-PYME\Ingresos tributarios-Impuestos a la renta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{A3ED3743-8E04-40C7-849C-D311898C7C02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1F2E8641-CC09-4EE2-8AB8-2E75C819BC7D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6252E9-5A21-4326-9F1E-323ECFE2B3CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{180C6776-FB6C-4163-ABDD-91AEF90E0C4F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{180C6776-FB6C-4163-ABDD-91AEF90E0C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="28" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="236">
   <si>
     <t>CONCEPTOS</t>
   </si>
@@ -743,18 +734,22 @@
   </si>
   <si>
     <t>millones usd</t>
+  </si>
+  <si>
+    <t>AÑO 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+    <numFmt numFmtId="167" formatCode="#,##0;\(#,##0\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -788,8 +783,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -808,8 +814,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -817,19 +829,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,99 +862,267 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{35B2ECE3-E3A4-4D86-9052-44B4CD91159C}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{2DAF8B79-F039-4C8D-BFB9-5BCF2DC62F6C}"/>
+    <cellStyle name="Normal 4" xfId="3" xr:uid="{44E76D2A-E594-409B-BAE6-418E08448CE8}"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="15">
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="166" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -951,231 +1144,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="167" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
+      <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1204,7 +1173,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Impuestos.xlsx]Hoja2!TablaDinámica1</c:name>
+    <c:name>[Ingresos Tributarios 2009-2019.xlsx]Hoja2!TablaDinámica1</c:name>
     <c:fmtId val="1"/>
   </c:pivotSource>
   <c:chart>
@@ -1252,7 +1221,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1308,7 +1277,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1364,7 +1333,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1420,7 +1389,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1476,7 +1445,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1532,7 +1501,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1588,7 +1557,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1644,7 +1613,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1700,7 +1669,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1756,7 +1725,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -1812,7 +1781,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
+              <a:endParaRPr lang="es-CL"/>
             </a:p>
           </c:txPr>
           <c:showLegendKey val="0"/>
@@ -3250,7 +3219,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1542517119"/>
@@ -3309,7 +3278,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1606300767"/>
@@ -3351,7 +3320,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-CL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3388,7 +3357,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-CL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4091,37 +4060,37 @@
     <cacheField name="CAT 05" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
-    <cacheField name="AÑO 2009" numFmtId="167">
+    <cacheField name="AÑO 2009" numFmtId="166">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-25086249.825994872" maxValue="27680502.149744365"/>
     </cacheField>
-    <cacheField name="AÑO 2010" numFmtId="167">
+    <cacheField name="AÑO 2010" numFmtId="166">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-27693828.208409" maxValue="30326825.920259997"/>
     </cacheField>
-    <cacheField name="AÑO 2011" numFmtId="167">
+    <cacheField name="AÑO 2011" numFmtId="166">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-32631500.396260001" maxValue="35372724.336337"/>
     </cacheField>
-    <cacheField name="AÑO 2012" numFmtId="167">
+    <cacheField name="AÑO 2012" numFmtId="166">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-36137151.081115" maxValue="39019406.930147998"/>
     </cacheField>
-    <cacheField name="AÑO 2013" numFmtId="167">
+    <cacheField name="AÑO 2013" numFmtId="166">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-37398467.052840002" maxValue="41137087.937550001"/>
     </cacheField>
-    <cacheField name="AÑO 2014" numFmtId="167">
+    <cacheField name="AÑO 2014" numFmtId="166">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="-40053305.559319995" maxValue="44245057.890288003"/>
     </cacheField>
-    <cacheField name="AÑO 2015" numFmtId="167">
+    <cacheField name="AÑO 2015" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-40534516.511016995" maxValue="45881017.089768"/>
     </cacheField>
-    <cacheField name="AÑO 2016" numFmtId="167">
+    <cacheField name="AÑO 2016" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-40820117.254334003" maxValue="47276749.238853"/>
     </cacheField>
-    <cacheField name="AÑO 2017" numFmtId="167">
+    <cacheField name="AÑO 2017" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-44789757.036958002" maxValue="51223968.082777001"/>
     </cacheField>
-    <cacheField name="AÑO 2018" numFmtId="167">
+    <cacheField name="AÑO 2018" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-52261924.578455001" maxValue="59364429.244549006"/>
     </cacheField>
-    <cacheField name="AÑO 2019" numFmtId="167">
+    <cacheField name="AÑO 2019" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-58347688.309561007" maxValue="66243707.959386013"/>
     </cacheField>
   </cacheFields>
@@ -7919,7 +7888,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56329D1F-53BF-4604-9336-BD09D6AF3774}" name="TablaDinámica1" cacheId="28" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{56329D1F-53BF-4604-9336-BD09D6AF3774}" name="TablaDinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" showDrill="0" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:M11" firstHeaderRow="0" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="19">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -8085,35 +8054,35 @@
         </ext>
       </extLst>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
         </ext>
       </extLst>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
         </ext>
       </extLst>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
         </ext>
       </extLst>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
         </ext>
       </extLst>
     </pivotField>
-    <pivotField dataField="1" compact="0" numFmtId="167" outline="0" showAll="0" defaultSubtotal="0">
+    <pivotField dataField="1" compact="0" numFmtId="166" outline="0" showAll="0" defaultSubtotal="0">
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
           <x14:pivotField fillDownLabels="1"/>
@@ -8211,7 +8180,7 @@
     <dataField name="Suma de AÑO 2019" fld="18" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="25">
+    <format dxfId="14">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -8428,9 +8397,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E372739-5A0A-4FBB-904B-B3F825548926}" name="Tabla1" displayName="Tabla1" ref="A2:S182" totalsRowShown="0" headerRowDxfId="29" dataDxfId="30" dataCellStyle="Millares">
-  <autoFilter ref="A2:S182" xr:uid="{4970BAE3-0C2F-46AE-AD5F-212D61E7E331}"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E372739-5A0A-4FBB-904B-B3F825548926}" name="Tabla1" displayName="Tabla1" ref="A2:T182" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" dataCellStyle="Millares">
+  <autoFilter ref="A2:T182" xr:uid="{4970BAE3-0C2F-46AE-AD5F-212D61E7E331}"/>
+  <tableColumns count="20">
     <tableColumn id="1" xr3:uid="{E958AFAA-0E16-4F7A-BE7E-73EEF4F65F49}" name="ID"/>
     <tableColumn id="19" xr3:uid="{D9DBE9EB-78C0-467E-BA1B-5FCCF82DD224}" name="Columna1"/>
     <tableColumn id="2" xr3:uid="{D270F92C-010C-4A4B-84A7-D578807413B9}" name="CONCEPTOS"/>
@@ -8439,17 +8408,18 @@
     <tableColumn id="5" xr3:uid="{C069F030-2EF9-456F-8124-BAA0965ADC51}" name="CAT 03"/>
     <tableColumn id="6" xr3:uid="{3FD99F7D-4ABD-4AC3-8CA4-8824D029567F}" name="CAT 04"/>
     <tableColumn id="7" xr3:uid="{2E1F1242-8CC3-41C1-BA51-E5E54A174E67}" name="CAT 05"/>
-    <tableColumn id="8" xr3:uid="{671A91EB-34EF-4B1F-BDF3-4E49F74EB657}" name="AÑO 2009" dataDxfId="41" dataCellStyle="Millares"/>
-    <tableColumn id="9" xr3:uid="{5B29E91D-900D-4A88-A527-34EAA7A0838C}" name="AÑO 2010" dataDxfId="40" dataCellStyle="Millares"/>
-    <tableColumn id="10" xr3:uid="{3A577F68-2177-4B5F-85E1-D5925858A3C3}" name="AÑO 2011" dataDxfId="39" dataCellStyle="Millares"/>
-    <tableColumn id="11" xr3:uid="{E4F55208-3203-4749-91EC-FAD2AD4ACA54}" name="AÑO 2012" dataDxfId="38" dataCellStyle="Millares"/>
-    <tableColumn id="12" xr3:uid="{B2614104-03CA-4160-B95F-95E203E0D514}" name="AÑO 2013" dataDxfId="37" dataCellStyle="Millares"/>
-    <tableColumn id="13" xr3:uid="{E6D69F0B-F616-4542-A391-1A7BCCC60B85}" name="AÑO 2014" dataDxfId="36" dataCellStyle="Millares"/>
-    <tableColumn id="14" xr3:uid="{C89ED862-1B36-4E9C-95D7-5B513527385F}" name="AÑO 2015" dataDxfId="35" dataCellStyle="Millares"/>
-    <tableColumn id="15" xr3:uid="{622599A1-04B9-4445-919F-FF1EA4390E7A}" name="AÑO 2016" dataDxfId="34" dataCellStyle="Millares"/>
-    <tableColumn id="16" xr3:uid="{13A5BFCF-0297-47D0-BA2D-2D071A0C9F21}" name="AÑO 2017" dataDxfId="33" dataCellStyle="Millares"/>
-    <tableColumn id="17" xr3:uid="{75FCDC5E-256B-4E30-BB5A-A7A9AF6EB9A4}" name="AÑO 2018" dataDxfId="32" dataCellStyle="Millares"/>
-    <tableColumn id="18" xr3:uid="{A762103E-C0F0-4CE7-ABDA-F4812B81C099}" name="AÑO 2019" dataDxfId="31" dataCellStyle="Millares"/>
+    <tableColumn id="8" xr3:uid="{671A91EB-34EF-4B1F-BDF3-4E49F74EB657}" name="AÑO 2009" dataDxfId="11" dataCellStyle="Millares"/>
+    <tableColumn id="9" xr3:uid="{5B29E91D-900D-4A88-A527-34EAA7A0838C}" name="AÑO 2010" dataDxfId="10" dataCellStyle="Millares"/>
+    <tableColumn id="10" xr3:uid="{3A577F68-2177-4B5F-85E1-D5925858A3C3}" name="AÑO 2011" dataDxfId="9" dataCellStyle="Millares"/>
+    <tableColumn id="11" xr3:uid="{E4F55208-3203-4749-91EC-FAD2AD4ACA54}" name="AÑO 2012" dataDxfId="8" dataCellStyle="Millares"/>
+    <tableColumn id="12" xr3:uid="{B2614104-03CA-4160-B95F-95E203E0D514}" name="AÑO 2013" dataDxfId="7" dataCellStyle="Millares"/>
+    <tableColumn id="13" xr3:uid="{E6D69F0B-F616-4542-A391-1A7BCCC60B85}" name="AÑO 2014" dataDxfId="6" dataCellStyle="Millares"/>
+    <tableColumn id="14" xr3:uid="{C89ED862-1B36-4E9C-95D7-5B513527385F}" name="AÑO 2015" dataDxfId="5" dataCellStyle="Millares"/>
+    <tableColumn id="15" xr3:uid="{622599A1-04B9-4445-919F-FF1EA4390E7A}" name="AÑO 2016" dataDxfId="4" dataCellStyle="Millares"/>
+    <tableColumn id="16" xr3:uid="{13A5BFCF-0297-47D0-BA2D-2D071A0C9F21}" name="AÑO 2017" dataDxfId="3" dataCellStyle="Millares"/>
+    <tableColumn id="17" xr3:uid="{75FCDC5E-256B-4E30-BB5A-A7A9AF6EB9A4}" name="AÑO 2018" dataDxfId="2" dataCellStyle="Millares"/>
+    <tableColumn id="18" xr3:uid="{A762103E-C0F0-4CE7-ABDA-F4812B81C099}" name="AÑO 2019" dataDxfId="1" dataCellStyle="Millares"/>
+    <tableColumn id="20" xr3:uid="{4F426752-3784-4282-BE8B-BA9C88F2B130}" name="AÑO 2020" dataDxfId="0" dataCellStyle="Millares"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8754,30 +8724,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBBFCBC-A046-46CB-A3C3-88C0352E3276}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="13" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>210</v>
       </c>
@@ -8818,7 +8788,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>211</v>
       </c>
@@ -8859,7 +8829,7 @@
         <v>14306908.946254015</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>212</v>
       </c>
@@ -8900,7 +8870,7 @@
         <v>16357282.799323363</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>213</v>
       </c>
@@ -8941,7 +8911,7 @@
         <v>2802132.086168</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>214</v>
       </c>
@@ -8982,7 +8952,7 @@
         <v>668211.20531500003</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>215</v>
       </c>
@@ -9023,7 +8993,7 @@
         <v>331846.27738331218</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>216</v>
       </c>
@@ -9064,7 +9034,7 @@
         <v>716223.1464301286</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>217</v>
       </c>
@@ -9105,7 +9075,7 @@
         <v>-453871.58426781528</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>218</v>
       </c>
@@ -9146,7 +9116,7 @@
         <v>-149510.49091299999</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G14" s="10">
         <v>18000000000000</v>
       </c>
@@ -9166,27 +9136,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFB2A666-6388-41BB-9922-8D57EF552987}">
-  <dimension ref="A2:S182"/>
+  <dimension ref="A2:T182"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" customWidth="1"/>
-    <col min="9" max="19" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.7109375" customWidth="1"/>
+    <col min="7" max="7" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
+    <col min="9" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>210</v>
       </c>
@@ -9244,8 +9216,11 @@
       <c r="S2" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T2" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>211</v>
       </c>
@@ -9299,8 +9274,11 @@
       <c r="S3" s="5">
         <v>9441521.9527115747</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T3" s="11">
+        <v>8967959.0552269947</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>211</v>
       </c>
@@ -9352,8 +9330,11 @@
       <c r="S4" s="5">
         <v>74108.590251000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T4" s="11">
+        <v>98563.343680999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>211</v>
       </c>
@@ -9405,8 +9386,11 @@
       <c r="S5" s="5">
         <v>587.65947275404346</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T5" s="11">
+        <v>409.12369800000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>211</v>
       </c>
@@ -9458,8 +9442,11 @@
       <c r="S6" s="5">
         <v>60690.449850000005</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T6" s="11">
+        <v>67866.934366999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>211</v>
       </c>
@@ -9511,8 +9498,11 @@
       <c r="S7" s="5">
         <v>3594.3163689999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T7" s="11">
+        <v>4610.3980570000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>211</v>
       </c>
@@ -9564,8 +9554,11 @@
       <c r="S8" s="5">
         <v>-171933.94641410452</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T8" s="5">
+        <v>-180829.02678053378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>211</v>
       </c>
@@ -9617,8 +9610,11 @@
       <c r="S9" s="5">
         <v>-450087.5083015252</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T9" s="5">
+        <v>-625953.77839256392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>211</v>
       </c>
@@ -9670,8 +9666,11 @@
       <c r="S10" s="5">
         <v>28.049355000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T10" s="13">
+        <v>19.000934000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>211</v>
       </c>
@@ -9723,8 +9722,11 @@
       <c r="S11" s="5">
         <v>17617.690711891242</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T11" s="13">
+        <v>123574.59647706023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>211</v>
       </c>
@@ -9776,8 +9778,11 @@
       <c r="S12" s="5">
         <v>2975835.9732399997</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T12" s="14">
+        <v>2994142.6547709992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>211</v>
       </c>
@@ -9829,8 +9834,11 @@
       <c r="S13" s="5">
         <v>269.25040099999995</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T13" s="14">
+        <v>21.260860000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>211</v>
       </c>
@@ -9882,8 +9890,11 @@
       <c r="S14" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T14" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>211</v>
       </c>
@@ -9935,8 +9946,11 @@
       <c r="S15" s="5">
         <v>10568.934652</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T15" s="15">
+        <v>19209.843714000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>211</v>
       </c>
@@ -9988,8 +10002,11 @@
       <c r="S16" s="5">
         <v>116.68271099999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T16" s="15">
+        <v>387.29939200000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>211</v>
       </c>
@@ -10041,8 +10058,11 @@
       <c r="S17" s="5">
         <v>22029.638466</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T17" s="15">
+        <v>27287.551079000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>211</v>
       </c>
@@ -10094,8 +10114,11 @@
       <c r="S18" s="5">
         <v>9549.967964999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T18" s="15">
+        <v>10028.593489999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>211</v>
       </c>
@@ -10147,8 +10170,11 @@
       <c r="S19" s="5">
         <v>-2576.9489290000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T19" s="5">
+        <v>-140.12090900000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>211</v>
       </c>
@@ -10200,8 +10226,11 @@
       <c r="S20" s="5">
         <v>798520.18752999976</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T20" s="16">
+        <v>1008362.494255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>211</v>
       </c>
@@ -10253,8 +10282,11 @@
       <c r="S21" s="5">
         <v>13946.395486000003</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T21" s="16">
+        <v>7971.8696240000027</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>211</v>
       </c>
@@ -10306,8 +10338,11 @@
       <c r="S22" s="5">
         <v>-890727.92002400011</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T22" s="5">
+        <v>-888848.31405000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>211</v>
       </c>
@@ -10359,8 +10394,11 @@
       <c r="S23" s="5">
         <v>-284760.30007599993</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T23" s="5">
+        <v>-279034.06068399997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>211</v>
       </c>
@@ -10412,8 +10450,11 @@
       <c r="S24" s="5">
         <v>730291.33620986994</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T24" s="17">
+        <v>614339.86089273833</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>211</v>
       </c>
@@ -10465,8 +10506,11 @@
       <c r="S25" s="5">
         <v>-41.213501000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T25" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>211</v>
       </c>
@@ -10518,8 +10562,11 @@
       <c r="S26" s="5">
         <v>444631.7476718562</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T26" s="17">
+        <v>243891.15040368197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>211</v>
       </c>
@@ -10571,8 +10618,11 @@
       <c r="S27" s="5">
         <v>715135.21265811613</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T27" s="17">
+        <v>671241.5760115186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>211</v>
       </c>
@@ -10624,8 +10674,11 @@
       <c r="S28" s="5">
         <v>240676.22064704372</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T28" s="17">
+        <v>261119.36400936291</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>211</v>
       </c>
@@ -10677,8 +10730,11 @@
       <c r="S29" s="5">
         <v>789.10883399999989</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T29" s="17">
+        <v>20700.940200758316</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>211</v>
       </c>
@@ -10730,8 +10786,11 @@
       <c r="S30" s="5">
         <v>322408.15804258257</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T30" s="17">
+        <v>493714.30615142849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>211</v>
       </c>
@@ -10780,8 +10839,11 @@
       <c r="S31" s="5">
         <v>122091.78819647482</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T31" s="17">
+        <v>203376.85150218636</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>211</v>
       </c>
@@ -10818,8 +10880,11 @@
       <c r="S32" s="5">
         <v>585.98587199999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T32" s="17">
+        <v>795137.47990512825</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>211</v>
       </c>
@@ -10868,8 +10933,11 @@
       <c r="S33" s="5">
         <v>285920.39617406175</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T33" s="17">
+        <v>174843.16117843645</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>211</v>
       </c>
@@ -10918,8 +10986,11 @@
       <c r="S34" s="5">
         <v>232869.53524329135</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T34" s="17">
+        <v>199401.91214685873</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>211</v>
       </c>
@@ -10968,8 +11039,11 @@
       <c r="S35" s="5">
         <v>32298.191577347745</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T35" s="5">
+        <v>-1137.6575819787452</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>211</v>
       </c>
@@ -11021,8 +11095,11 @@
       <c r="S36" s="5">
         <v>-8771872.1576368827</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T36" s="5">
+        <v>-9292889.2429593969</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>211</v>
       </c>
@@ -11074,8 +11151,11 @@
       <c r="S37" s="5">
         <v>-1150582.4018864576</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T37" s="5">
+        <v>-979709.6762295767</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>211</v>
       </c>
@@ -11127,8 +11207,11 @@
       <c r="S38" s="5">
         <v>-54134.025332999998</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T38" s="5">
+        <v>-25799.869563</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>211</v>
       </c>
@@ -11180,8 +11263,11 @@
       <c r="S39" s="5">
         <v>-15150.960144000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T39" s="5">
+        <v>-17155.776034999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>211</v>
       </c>
@@ -11233,8 +11319,11 @@
       <c r="S40" s="5">
         <v>-3883.4325220000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T40" s="5">
+        <v>-4831.2808480000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>211</v>
       </c>
@@ -11276,8 +11365,11 @@
       <c r="S41" s="5">
         <v>-1047.4714547446104</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T41" s="5">
+        <v>-928.72030018800876</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>211</v>
       </c>
@@ -11329,8 +11421,11 @@
       <c r="S42" s="5">
         <v>-98375.118089000011</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T42" s="5">
+        <v>-115895.707862</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>211</v>
       </c>
@@ -11385,8 +11480,11 @@
       <c r="S43" s="5">
         <v>-71424.637887999983</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T43" s="5">
+        <v>-79001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>211</v>
       </c>
@@ -11441,8 +11539,11 @@
       <c r="S44" s="5">
         <v>62383.875814000014</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T44" s="5">
+        <v>64512</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>211</v>
       </c>
@@ -11494,8 +11595,11 @@
       <c r="S45" s="5">
         <v>-3452.0077909999995</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T45" s="5">
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>211</v>
       </c>
@@ -11547,8 +11651,11 @@
       <c r="S46" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T46" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>211</v>
       </c>
@@ -11600,8 +11707,11 @@
       <c r="S47" s="5">
         <v>-13930.070325000001</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T47" s="5">
+        <v>-16778</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>211</v>
       </c>
@@ -11653,8 +11763,11 @@
       <c r="S48" s="5">
         <v>-7042.6246750000009</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T48" s="5">
+        <v>-6601</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>211</v>
       </c>
@@ -11706,8 +11819,11 @@
       <c r="S49" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T49" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>211</v>
       </c>
@@ -11759,8 +11875,11 @@
       <c r="S50" s="5">
         <v>3889069.8855990036</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T50" s="5">
+        <v>4611475</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>211</v>
       </c>
@@ -11812,8 +11931,11 @@
       <c r="S51" s="5">
         <v>-4178361.7914636726</v>
       </c>
-    </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T51" s="5">
+        <v>-4919419</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>211</v>
       </c>
@@ -11865,8 +11987,11 @@
       <c r="S52" s="5">
         <v>47781.797371796041</v>
       </c>
-    </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T52" s="5">
+        <v>39516</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>211</v>
       </c>
@@ -11921,8 +12046,11 @@
       <c r="S53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T53" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>211</v>
       </c>
@@ -11977,8 +12105,11 @@
       <c r="S54" s="5">
         <v>-102.94694300000002</v>
       </c>
-    </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T54" s="5">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>211</v>
       </c>
@@ -12030,8 +12161,11 @@
       <c r="S55" s="5">
         <v>7184652.6569990003</v>
       </c>
-    </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T55" s="5">
+        <v>5521745</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>211</v>
       </c>
@@ -12083,8 +12217,11 @@
       <c r="S56" s="5">
         <v>1550960.3854891486</v>
       </c>
-    </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T56" s="5">
+        <v>1625319</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>211</v>
       </c>
@@ -12139,8 +12276,11 @@
       <c r="S57" s="5">
         <v>667326.20964499994</v>
       </c>
-    </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T57" s="5">
+        <v>672693</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>211</v>
       </c>
@@ -12195,8 +12335,11 @@
       <c r="S58" s="5">
         <v>96957.66840699999</v>
       </c>
-    </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T58" s="5">
+        <v>86345</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>211</v>
       </c>
@@ -12248,8 +12391,11 @@
       <c r="S59" s="5">
         <v>30347.891503999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T59" s="5">
+        <v>25784</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>211</v>
       </c>
@@ -12301,8 +12447,11 @@
       <c r="S60" s="5">
         <v>16382.997343999999</v>
       </c>
-    </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T60" s="5">
+        <v>16877</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>211</v>
       </c>
@@ -12357,8 +12506,11 @@
       <c r="S61" s="5">
         <v>106646.10839094</v>
       </c>
-    </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T61" s="5">
+        <v>96556</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>211</v>
       </c>
@@ -12413,8 +12565,11 @@
       <c r="S62" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T62" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>211</v>
       </c>
@@ -12469,8 +12624,11 @@
       <c r="S63" s="5">
         <v>18768.731351999755</v>
       </c>
-    </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T63" s="5">
+        <v>10189</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>211</v>
       </c>
@@ -12525,8 +12683,11 @@
       <c r="S64" s="5">
         <v>-2305.1666320001427</v>
       </c>
-    </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T64" s="5">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>211</v>
       </c>
@@ -12581,8 +12742,11 @@
       <c r="S65" s="5">
         <v>215868.0955468374</v>
       </c>
-    </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T65" s="5">
+        <v>249688</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>211</v>
       </c>
@@ -12637,8 +12801,11 @@
       <c r="S66" s="5">
         <v>-90.769918000000104</v>
       </c>
-    </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T66" s="5">
+        <v>-99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>211</v>
       </c>
@@ -12693,8 +12860,11 @@
       <c r="S67" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T67" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>211</v>
       </c>
@@ -12749,8 +12919,11 @@
       <c r="S68" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T68" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>211</v>
       </c>
@@ -12802,8 +12975,11 @@
       <c r="S69" s="5">
         <v>723.71551999999997</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T69" s="5">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>211</v>
       </c>
@@ -12855,8 +13031,11 @@
       <c r="S70" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>211</v>
       </c>
@@ -12908,8 +13087,11 @@
       <c r="S71" s="5">
         <v>42532.759685607925</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T71" s="5">
+        <v>33055</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>211</v>
       </c>
@@ -12958,8 +13140,11 @@
       <c r="S72" s="5">
         <v>-23115.35494443772</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T72" s="5">
+        <v>-145265</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>211</v>
       </c>
@@ -13008,8 +13193,11 @@
       <c r="S73" s="5">
         <v>-1418.6134213600001</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T73" s="5">
+        <v>-12757</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>211</v>
       </c>
@@ -13055,8 +13243,11 @@
       <c r="S74" s="5">
         <v>16240.135599999998</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T74" s="5">
+        <v>48174</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>212</v>
       </c>
@@ -13108,8 +13299,11 @@
       <c r="S75" s="5">
         <v>55723977.143357992</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T75" s="5">
+        <v>56499605</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>212</v>
       </c>
@@ -13161,8 +13355,11 @@
       <c r="S76" s="5">
         <v>-49172053.146743998</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T76" s="5">
+        <v>-49811223</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>212</v>
       </c>
@@ -13217,8 +13414,11 @@
       <c r="S77" s="5">
         <v>194070.41776399998</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T77" s="5">
+        <v>199282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>212</v>
       </c>
@@ -13273,8 +13473,11 @@
       <c r="S78" s="5">
         <v>30571.415207000002</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T78" s="5">
+        <v>31774</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>212</v>
       </c>
@@ -13329,8 +13532,11 @@
       <c r="S79" s="5">
         <v>34269.255739</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T79" s="5">
+        <v>34750</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>212</v>
       </c>
@@ -13385,8 +13591,11 @@
       <c r="S80" s="5">
         <v>-5226.6395140000004</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T80" s="5">
+        <v>-4090</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>212</v>
       </c>
@@ -13438,8 +13647,11 @@
       <c r="S81" s="5">
         <v>464.776275</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T81" s="5">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>212</v>
       </c>
@@ -13491,8 +13703,11 @@
       <c r="S82" s="5">
         <v>-2748.3047330000049</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T82" s="5">
+        <v>-7980</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>212</v>
       </c>
@@ -13544,8 +13759,11 @@
       <c r="S83" s="5">
         <v>275755.36979099998</v>
       </c>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T83" s="5">
+        <v>163038</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>212</v>
       </c>
@@ -13597,8 +13815,11 @@
       <c r="S84" s="5">
         <v>112521.15552199999</v>
       </c>
-    </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T84" s="5">
+        <v>-180593</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>212</v>
       </c>
@@ -13650,8 +13871,11 @@
       <c r="S85" s="5">
         <v>8534679.6106109992</v>
       </c>
-    </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T85" s="5">
+        <v>8143829</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>212</v>
       </c>
@@ -13703,8 +13927,11 @@
       <c r="S86" s="5">
         <v>17749.468140000004</v>
       </c>
-    </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T86" s="5">
+        <v>21045</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>212</v>
       </c>
@@ -13756,8 +13983,11 @@
       <c r="S87" s="5">
         <v>68.895566000000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T87" s="5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>212</v>
       </c>
@@ -13815,8 +14045,11 @@
       <c r="S88" s="5">
         <v>141414.6801</v>
       </c>
-    </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T88" s="5">
+        <v>152665</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>212</v>
       </c>
@@ -13874,8 +14107,11 @@
       <c r="S89" s="5">
         <v>-76393.646693999995</v>
       </c>
-    </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T89" s="5">
+        <v>-80310</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>212</v>
       </c>
@@ -13933,8 +14169,11 @@
       <c r="S90" s="5">
         <v>150150.72227699999</v>
       </c>
-    </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T90" s="5">
+        <v>153260</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>212</v>
       </c>
@@ -13992,8 +14231,11 @@
       <c r="S91" s="5">
         <v>-69056.040378999998</v>
       </c>
-    </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T91" s="5">
+        <v>-71127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>212</v>
       </c>
@@ -14051,8 +14293,11 @@
       <c r="S92" s="5">
         <v>193220.346662</v>
       </c>
-    </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T92" s="5">
+        <v>198488</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>212</v>
       </c>
@@ -14110,8 +14355,11 @@
       <c r="S93" s="5">
         <v>-48107.929708999996</v>
       </c>
-    </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T93" s="5">
+        <v>-56217</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>212</v>
       </c>
@@ -14169,8 +14417,11 @@
       <c r="S94" s="5">
         <v>197858.699162</v>
       </c>
-    </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T94" s="5">
+        <v>217078</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>212</v>
       </c>
@@ -14228,8 +14479,11 @@
       <c r="S95" s="5">
         <v>-70475.741045999996</v>
       </c>
-    </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T95" s="5">
+        <v>-73635</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>212</v>
       </c>
@@ -14287,8 +14541,11 @@
       <c r="S96" s="5">
         <v>2978.6060300000004</v>
       </c>
-    </row>
-    <row r="97" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T96" s="5">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>212</v>
       </c>
@@ -14346,8 +14603,11 @@
       <c r="S97" s="5">
         <v>-1014.877168</v>
       </c>
-    </row>
-    <row r="98" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T97" s="5">
+        <v>-753</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>212</v>
       </c>
@@ -14402,8 +14662,11 @@
       <c r="S98" s="5">
         <v>21.806748999999996</v>
       </c>
-    </row>
-    <row r="99" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T98" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>212</v>
       </c>
@@ -14458,8 +14721,11 @@
       <c r="S99" s="5">
         <v>0.98464799999999997</v>
       </c>
-    </row>
-    <row r="100" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>212</v>
       </c>
@@ -14514,8 +14780,11 @@
       <c r="S100" s="5">
         <v>69980.89069</v>
       </c>
-    </row>
-    <row r="101" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T100" s="5">
+        <v>62982</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>212</v>
       </c>
@@ -14570,8 +14839,11 @@
       <c r="S101" s="5">
         <v>-63.865493999999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T101" s="5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>212</v>
       </c>
@@ -14626,8 +14898,11 @@
       <c r="S102" s="5">
         <v>-0.93908199999999997</v>
       </c>
-    </row>
-    <row r="103" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T102" s="5">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>212</v>
       </c>
@@ -14682,8 +14957,11 @@
       <c r="S103" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T103" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>212</v>
       </c>
@@ -14738,8 +15016,11 @@
       <c r="S104" s="5">
         <v>-46876.405975999995</v>
       </c>
-    </row>
-    <row r="105" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T104" s="5">
+        <v>-38062</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>212</v>
       </c>
@@ -14791,8 +15072,11 @@
       <c r="S105" s="5">
         <v>66243707.959386013</v>
       </c>
-    </row>
-    <row r="106" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T105" s="5">
+        <v>73314154</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>212</v>
       </c>
@@ -14844,8 +15128,11 @@
       <c r="S106" s="5">
         <v>-58347688.309561007</v>
       </c>
-    </row>
-    <row r="107" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T106" s="5">
+        <v>-64666644</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>212</v>
       </c>
@@ -14897,8 +15184,11 @@
       <c r="S107" s="5">
         <v>196396.70879400003</v>
       </c>
-    </row>
-    <row r="108" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T107" s="5">
+        <v>-177</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>212</v>
       </c>
@@ -14948,8 +15238,11 @@
       <c r="S108" s="5">
         <v>-415811.70233400003</v>
       </c>
-    </row>
-    <row r="109" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T108" s="5">
+        <v>-314552</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>212</v>
       </c>
@@ -14998,8 +15291,11 @@
       <c r="S109" s="5">
         <v>-329189.16605400003</v>
       </c>
-    </row>
-    <row r="110" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T109" s="5">
+        <v>-390458</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>212</v>
       </c>
@@ -15051,8 +15347,11 @@
       <c r="S110" s="5">
         <v>-1106296.688015</v>
       </c>
-    </row>
-    <row r="111" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T110" s="5">
+        <v>-1003632</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>212</v>
       </c>
@@ -15104,8 +15403,11 @@
       <c r="S111" s="5">
         <v>-5696115.0194359999</v>
       </c>
-    </row>
-    <row r="112" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T111" s="5">
+        <v>-6087600</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>212</v>
       </c>
@@ -15157,8 +15459,11 @@
       <c r="S112" s="5">
         <v>-6015.0625019999998</v>
       </c>
-    </row>
-    <row r="113" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T112" s="5">
+        <v>-5520</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>212</v>
       </c>
@@ -15210,8 +15515,11 @@
       <c r="S113" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T113" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>212</v>
       </c>
@@ -15263,8 +15571,11 @@
       <c r="S114" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T114" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>212</v>
       </c>
@@ -15313,8 +15624,11 @@
       <c r="S115" s="5">
         <v>-331784.43331500003</v>
       </c>
-    </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T115" s="5">
+        <v>-453957</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>212</v>
       </c>
@@ -15363,8 +15677,11 @@
       <c r="S116" s="5">
         <v>-43.754077000000002</v>
       </c>
-    </row>
-    <row r="117" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T116" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>212</v>
       </c>
@@ -15413,8 +15730,11 @@
       <c r="S117" s="5">
         <v>-35198.964408</v>
       </c>
-    </row>
-    <row r="118" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T117" s="5">
+        <v>-45804</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>212</v>
       </c>
@@ -15460,8 +15780,11 @@
       <c r="S118" s="5">
         <v>-2415.4769066399999</v>
       </c>
-    </row>
-    <row r="119" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T118" s="5">
+        <v>-21721</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>213</v>
       </c>
@@ -15510,8 +15833,11 @@
       <c r="S119" s="5">
         <v>941385.61929000006</v>
       </c>
-    </row>
-    <row r="120" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T119" s="5">
+        <v>974335</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>213</v>
       </c>
@@ -15560,8 +15886,11 @@
       <c r="S120" s="5">
         <v>31950.333168000001</v>
       </c>
-    </row>
-    <row r="121" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T120" s="5">
+        <v>47581</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>213</v>
       </c>
@@ -15610,8 +15939,11 @@
       <c r="S121" s="5">
         <v>2884.2042940000001</v>
       </c>
-    </row>
-    <row r="122" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T121" s="5">
+        <v>2152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>213</v>
       </c>
@@ -15663,8 +15995,11 @@
       <c r="S122" s="5">
         <v>117146.29496300001</v>
       </c>
-    </row>
-    <row r="123" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T122" s="5">
+        <v>149155</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>213</v>
       </c>
@@ -15716,8 +16051,11 @@
       <c r="S123" s="5">
         <v>1321126.6894669998</v>
       </c>
-    </row>
-    <row r="124" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T123" s="5">
+        <v>1160037</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>213</v>
       </c>
@@ -15769,8 +16107,11 @@
       <c r="S124" s="5">
         <v>448950.27757000003</v>
       </c>
-    </row>
-    <row r="125" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T124" s="5">
+        <v>660129</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>213</v>
       </c>
@@ -15822,8 +16163,11 @@
       <c r="S125" s="5">
         <v>360173.50316999998</v>
       </c>
-    </row>
-    <row r="126" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T125" s="5">
+        <v>381019</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>213</v>
       </c>
@@ -15875,8 +16219,11 @@
       <c r="S126" s="5">
         <v>-379431.85931999999</v>
       </c>
-    </row>
-    <row r="127" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T126" s="5">
+        <v>-471172</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>213</v>
       </c>
@@ -15928,8 +16275,11 @@
       <c r="S127" s="5">
         <v>-65970.971028</v>
       </c>
-    </row>
-    <row r="128" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T127" s="5">
+        <v>-85086</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>213</v>
       </c>
@@ -15978,8 +16328,11 @@
       <c r="S128" s="5">
         <v>5806.5977940000002</v>
       </c>
-    </row>
-    <row r="129" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T128" s="5">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>213</v>
       </c>
@@ -16028,8 +16381,11 @@
       <c r="S129" s="5">
         <v>448.94069000000002</v>
       </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T129" s="5">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>213</v>
       </c>
@@ -16075,8 +16431,11 @@
       <c r="S130" s="5">
         <v>17662.456110000003</v>
       </c>
-    </row>
-    <row r="131" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T130" s="5">
+        <v>33104</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>214</v>
       </c>
@@ -16122,8 +16481,11 @@
       <c r="S131" s="5">
         <v>546678.00755700003</v>
       </c>
-    </row>
-    <row r="132" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T131" s="5">
+        <v>306262</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>214</v>
       </c>
@@ -16169,8 +16531,11 @@
       <c r="S132" s="5">
         <v>9600.9472190000015</v>
       </c>
-    </row>
-    <row r="133" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T132" s="5">
+        <v>6707</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>214</v>
       </c>
@@ -16216,8 +16581,11 @@
       <c r="S133" s="5">
         <v>74.239407</v>
       </c>
-    </row>
-    <row r="134" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T133" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>214</v>
       </c>
@@ -16263,8 +16631,11 @@
       <c r="S134" s="5">
         <v>113556.18987799999</v>
       </c>
-    </row>
-    <row r="135" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T134" s="5">
+        <v>41013</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>214</v>
       </c>
@@ -16310,8 +16681,11 @@
       <c r="S135" s="5">
         <v>348.84789699999999</v>
       </c>
-    </row>
-    <row r="136" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T135" s="5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>214</v>
       </c>
@@ -16357,8 +16731,11 @@
       <c r="S136" s="5">
         <v>-4344.1458400000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T136" s="5">
+        <v>-3633</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>214</v>
       </c>
@@ -16404,8 +16781,11 @@
       <c r="S137" s="5">
         <v>2297.119197</v>
       </c>
-    </row>
-    <row r="138" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T137" s="5">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>215</v>
       </c>
@@ -16454,8 +16834,11 @@
       <c r="S138" s="5">
         <v>4.4921999999999995</v>
       </c>
-    </row>
-    <row r="139" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T138" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>215</v>
       </c>
@@ -16504,8 +16887,11 @@
       <c r="S139" s="5">
         <v>349052.11124600004</v>
       </c>
-    </row>
-    <row r="140" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T139" s="5">
+        <v>343026</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>215</v>
       </c>
@@ -16554,8 +16940,11 @@
       <c r="S140" s="5">
         <v>3875.2915353121302</v>
       </c>
-    </row>
-    <row r="141" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T140" s="5">
+        <v>-24021</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>215</v>
       </c>
@@ -16604,8 +16993,11 @@
       <c r="S141" s="5">
         <v>-17811.962746999998</v>
       </c>
-    </row>
-    <row r="142" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T141" s="5">
+        <v>-21964</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>215</v>
       </c>
@@ -16654,8 +17046,11 @@
       <c r="S142" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="143" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T142" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>215</v>
       </c>
@@ -16704,8 +17099,11 @@
       <c r="S143" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="144" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T143" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>215</v>
       </c>
@@ -16754,8 +17152,11 @@
       <c r="S144" s="5">
         <v>-18.973935999999998</v>
       </c>
-    </row>
-    <row r="145" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T144" s="5">
+        <v>-104</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>215</v>
       </c>
@@ -16804,8 +17205,11 @@
       <c r="S145" s="5">
         <v>-3254.6809149999999</v>
       </c>
-    </row>
-    <row r="146" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T145" s="5">
+        <v>-3225</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>215</v>
       </c>
@@ -16854,8 +17258,11 @@
       <c r="S146" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T146" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>216</v>
       </c>
@@ -16904,8 +17311,11 @@
       <c r="S147" s="5">
         <v>50438.144709</v>
       </c>
-    </row>
-    <row r="148" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T147" s="5">
+        <v>128692</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>216</v>
       </c>
@@ -16954,8 +17364,11 @@
       <c r="S148" s="5">
         <v>12385.810143000002</v>
       </c>
-    </row>
-    <row r="149" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T148" s="5">
+        <v>26740</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>216</v>
       </c>
@@ -17001,8 +17414,11 @@
       <c r="S149" s="5">
         <v>54695.632885999999</v>
       </c>
-    </row>
-    <row r="150" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T149" s="5">
+        <v>54932</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>216</v>
       </c>
@@ -17051,8 +17467,11 @@
       <c r="S150" s="5">
         <v>31728.321151999997</v>
       </c>
-    </row>
-    <row r="151" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T150" s="5">
+        <v>25093</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>216</v>
       </c>
@@ -17101,8 +17520,11 @@
       <c r="S151" s="5">
         <v>21175.175310000002</v>
       </c>
-    </row>
-    <row r="152" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T151" s="5">
+        <v>6729</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>216</v>
       </c>
@@ -17151,8 +17573,11 @@
       <c r="S152" s="5">
         <v>6060.1827279999998</v>
       </c>
-    </row>
-    <row r="153" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T152" s="5">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>216</v>
       </c>
@@ -17201,8 +17626,11 @@
       <c r="S153" s="5">
         <v>54170.023352000004</v>
       </c>
-    </row>
-    <row r="154" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T153" s="5">
+        <v>16700</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>216</v>
       </c>
@@ -17248,8 +17676,11 @@
       <c r="S154" s="5">
         <v>198.12453100000002</v>
       </c>
-    </row>
-    <row r="155" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T154" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>216</v>
       </c>
@@ -17295,8 +17726,11 @@
       <c r="S155" s="5">
         <v>23455.272078999998</v>
       </c>
-    </row>
-    <row r="156" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T155" s="5">
+        <v>23767</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>216</v>
       </c>
@@ -17342,8 +17776,11 @@
       <c r="S156" s="5">
         <v>214226.60092767113</v>
       </c>
-    </row>
-    <row r="157" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T156" s="5">
+        <v>205888</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>216</v>
       </c>
@@ -17389,8 +17826,11 @@
       <c r="S157" s="5">
         <v>-3.8677620000000004</v>
       </c>
-    </row>
-    <row r="158" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T157" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>216</v>
       </c>
@@ -17439,8 +17879,11 @@
       <c r="S158" s="5">
         <v>12050.766520000001</v>
       </c>
-    </row>
-    <row r="159" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T158" s="5">
+        <v>5324</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>216</v>
       </c>
@@ -17492,8 +17935,11 @@
       <c r="S159" s="5">
         <v>378562.81066259864</v>
       </c>
-    </row>
-    <row r="160" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T159" s="5">
+        <v>162434</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>216</v>
       </c>
@@ -17545,8 +17991,11 @@
       <c r="S160" s="5">
         <v>-277653.16761945118</v>
       </c>
-    </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T160" s="5">
+        <v>-75457</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>216</v>
       </c>
@@ -17598,8 +18047,11 @@
       <c r="S161" s="5">
         <v>-130602.49187199998</v>
       </c>
-    </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T161" s="5">
+        <v>-92091</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>216</v>
       </c>
@@ -17648,8 +18100,11 @@
       <c r="S162" s="5">
         <v>52412.407383310245</v>
       </c>
-    </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T162" s="5">
+        <v>29278</v>
+      </c>
+    </row>
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>216</v>
       </c>
@@ -17698,8 +18153,11 @@
       <c r="S163" s="5">
         <v>4393.4930110000005</v>
       </c>
-    </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T163" s="5">
+        <v>1616</v>
+      </c>
+    </row>
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>216</v>
       </c>
@@ -17748,8 +18206,11 @@
       <c r="S164" s="5">
         <v>63.893607999999993</v>
       </c>
-    </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T164" s="5">
+        <v>-172</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>216</v>
       </c>
@@ -17798,8 +18259,11 @@
       <c r="S165" s="5">
         <v>-19017.878231999999</v>
       </c>
-    </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T165" s="5">
+        <v>-7640</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>216</v>
       </c>
@@ -17848,8 +18312,11 @@
       <c r="S166" s="5">
         <v>2073.1867979999988</v>
       </c>
-    </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T166" s="5">
+        <v>-11794</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>216</v>
       </c>
@@ -17898,8 +18365,11 @@
       <c r="S167" s="5">
         <v>8307.4882799999996</v>
       </c>
-    </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T167" s="5">
+        <v>7314</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>216</v>
       </c>
@@ -17948,8 +18418,11 @@
       <c r="S168" s="5">
         <v>3246.4513419999994</v>
       </c>
-    </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T168" s="5">
+        <v>-9109</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>216</v>
       </c>
@@ -17986,8 +18459,11 @@
       <c r="S169" s="5">
         <v>-3322.5954960002564</v>
       </c>
-    </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T169" s="5">
+        <v>-39101</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>216</v>
       </c>
@@ -18031,13 +18507,14 @@
         <v>95841.708374000009</v>
       </c>
       <c r="R170" s="5">
-        <v>217064.31626699996</v>
+        <v>217179.36198899997</v>
       </c>
       <c r="S170" s="5">
         <v>217179.36198899997</v>
       </c>
-    </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T170" s="12"/>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>217</v>
       </c>
@@ -18086,8 +18563,11 @@
       <c r="S171" s="5">
         <v>-979.87860499999988</v>
       </c>
-    </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T171" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>217</v>
       </c>
@@ -18136,8 +18616,11 @@
       <c r="S172" s="5">
         <v>118.61679300000003</v>
       </c>
-    </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T172" s="5">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>217</v>
       </c>
@@ -18186,8 +18669,11 @@
       <c r="S173" s="5">
         <v>-862660.9522538539</v>
       </c>
-    </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T173" s="5">
+        <v>-662910</v>
+      </c>
+    </row>
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>217</v>
       </c>
@@ -18236,8 +18722,11 @@
       <c r="S174" s="5">
         <v>-5224.0435230000003</v>
       </c>
-    </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T174" s="5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>217</v>
       </c>
@@ -18286,8 +18775,11 @@
       <c r="S175" s="5">
         <v>-69466.368832999986</v>
       </c>
-    </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T175" s="5">
+        <v>-40224</v>
+      </c>
+    </row>
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>217</v>
       </c>
@@ -18336,8 +18828,11 @@
       <c r="S176" s="5">
         <v>-1390.600369</v>
       </c>
-    </row>
-    <row r="177" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T176" s="5">
+        <v>-3541</v>
+      </c>
+    </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>217</v>
       </c>
@@ -18386,8 +18881,11 @@
       <c r="S177" s="5">
         <v>-137.951075</v>
       </c>
-    </row>
-    <row r="178" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T177" s="5">
+        <v>-28</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>217</v>
       </c>
@@ -18436,8 +18934,11 @@
       <c r="S178" s="5">
         <v>-129.803057</v>
       </c>
-    </row>
-    <row r="179" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T178" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>217</v>
       </c>
@@ -18486,8 +18987,11 @@
       <c r="S179" s="5">
         <v>478035.25329103856</v>
       </c>
-    </row>
-    <row r="180" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T179" s="5">
+        <v>395219</v>
+      </c>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>217</v>
       </c>
@@ -18536,8 +19040,11 @@
       <c r="S180" s="5">
         <v>7964.5291460000017</v>
       </c>
-    </row>
-    <row r="181" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T180" s="5">
+        <v>15338</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>217</v>
       </c>
@@ -18586,8 +19093,11 @@
       <c r="S181" s="5">
         <v>-0.38578199999999996</v>
       </c>
-    </row>
-    <row r="182" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T181" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>218</v>
       </c>
@@ -18632,6 +19142,9 @@
       </c>
       <c r="S182" s="5">
         <v>-149510.49091299999</v>
+      </c>
+      <c r="T182" s="5">
+        <v>-58547</v>
       </c>
     </row>
   </sheetData>

</xml_diff>